<commit_message>
Updated Excel files and license
The first page of the template was updated and a license file added.
</commit_message>
<xml_diff>
--- a/Economics/System-Scale Cost Database.xlsx
+++ b/Economics/System-Scale Cost Database.xlsx
@@ -1,32 +1,500 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sclo\Documents\GitHub\Scale-Coupled-Open-Innovation-Network\Economics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3073A1E6-054A-4F0B-9F9F-871BB562253B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-103" yWindow="497" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TEA data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Schalk Cloete</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{3E297B5B-C11C-4D9A-9D16-9B005BD0F52E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+A distinctive name (plus an acronym, if needed) by which this process should be identified in future works.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{74AC91DF-AB7C-4944-B241-8812BA090454}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Version of the SEA tool used for the assessment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{782B7EB3-655E-43DA-9B9F-4AC12660F16C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Year selected in the SEA tool</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{E2AC20E4-8349-461B-9F21-F6E25576B119}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Region selected for the assessment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{022843D0-33F1-4475-99EF-06962DBF3DD6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+E.g., hydrogen, electricity, ammonia, etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{51B910DF-CD19-42F6-AA71-28F5969F76E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Total Capital Requirement from the SEA Tool</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{47A65FCA-6400-46AE-B32D-5D675D7727E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+E.g., €/kWe</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{BAC463F3-E19C-4CD2-BC41-8BA78F1DA431}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+E.g., LHV natural gas input. It should be consistent with the product and fuel  selected in columns E &amp; N.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{2092EC9F-7554-4BDD-B564-06F523444905}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+E.g., %CAPEX/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{95579A01-5F73-417F-B596-5E15721C073D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Excluding fuel</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{AD24B076-FC58-4CE3-9467-341CFB0F3C3E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+E.g., €/MWh</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{11ACBB61-2720-4171-9C3C-2BFAFB052837}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Natural gas, coal, biomass, hydrogen, etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{4AA80A1F-95FC-40B4-8D92-59EDB485F6EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schalk Cloete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Published paper linked to these numbers</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Process concepts assessed using the SEA Tool</t>
+  </si>
+  <si>
+    <t>Capital cost</t>
+  </si>
+  <si>
+    <t>Capital cost unit</t>
+  </si>
+  <si>
+    <t>Efficiency basis</t>
+  </si>
+  <si>
+    <t>Efficiency (%)</t>
+  </si>
+  <si>
+    <t>Fixed O&amp;M</t>
+  </si>
+  <si>
+    <t>Fixed O&amp;M unit</t>
+  </si>
+  <si>
+    <t>Variable O&amp;M</t>
+  </si>
+  <si>
+    <t>Variable O&amp;M unit</t>
+  </si>
+  <si>
+    <t>Fuel type</t>
+  </si>
+  <si>
+    <t>Lifetime (years)</t>
+  </si>
+  <si>
+    <t>Cost year</t>
+  </si>
+  <si>
+    <t>SEA tool version</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Process name (and acronym)</t>
+  </si>
+  <si>
+    <r>
+      <t>CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>₂</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> avoidance (%)</t>
+    </r>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +505,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,14 +513,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +822,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="50.69140625" customWidth="1"/>
+    <col min="2" max="16" width="15.69140625" customWidth="1"/>
+    <col min="17" max="17" width="50.69140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>